<commit_message>
Starting to work through issues to get the standard functionality back
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3906EDC-8967-4373-92C5-A854A0A7F95E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,57 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Priority (1-5)</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Affected vi(s)</t>
+  </si>
+  <si>
+    <t>\Plugins\Utility\Full Build Assert.vi
+\Plugins\Utility\Set Assert VI UID.vi
+\Plugins\Utility\Add Evaluation String</t>
+  </si>
+  <si>
+    <t>Issue_001</t>
+  </si>
+  <si>
+    <t>Useless naming of object references</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Issue_002</t>
+  </si>
+  <si>
+    <t>Changes to "Inline or Forked.vi" broke calling code</t>
+  </si>
+  <si>
+    <t>In work</t>
+  </si>
+  <si>
+    <t>\Plugins\Utility\Inline or Forked.vi</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +383,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sorting out a bug in Inline or Forked.vi and the calling code where the wrong sub-vi reference was being passed. I think it should work now...
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3906EDC-8967-4373-92C5-A854A0A7F95E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AD1926-F84B-4D25-BCF9-9E19B20DB3AC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>\Plugins\Utility\Inline or Forked.vi</t>
+  </si>
+  <si>
+    <t>Issue_003</t>
+  </si>
+  <si>
+    <t>Right click plugin isn't appearing</t>
+  </si>
+  <si>
+    <t>Solved</t>
+  </si>
+  <si>
+    <t>added in the code to translate the wire type to the new one required by the "Inline or Forked.vi". Now appears to be working.</t>
   </si>
 </sst>
 </file>
@@ -384,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,7 +409,7 @@
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="147.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -448,10 +460,27 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Issue_002 and Issue_003. Created about 8 new issues in the spreadsheet
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AD1926-F84B-4D25-BCF9-9E19B20DB3AC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C2B0C8-5CF9-420F-9FDF-088EB61D6864}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4185" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$11</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -60,9 +63,6 @@
     <t>Changes to "Inline or Forked.vi" broke calling code</t>
   </si>
   <si>
-    <t>In work</t>
-  </si>
-  <si>
     <t>\Plugins\Utility\Inline or Forked.vi</t>
   </si>
   <si>
@@ -76,6 +76,72 @@
   </si>
   <si>
     <t>added in the code to translate the wire type to the new one required by the "Inline or Forked.vi". Now appears to be working.</t>
+  </si>
+  <si>
+    <t>Issue_004</t>
+  </si>
+  <si>
+    <t>Asserts aren't being added to the wires correctly when inside a structure</t>
+  </si>
+  <si>
+    <t>I think its for both inline and forked asserts being added. When its inside a structure, the object reference is coming through as invalid.</t>
+  </si>
+  <si>
+    <t>Issue_005</t>
+  </si>
+  <si>
+    <t>Default to the main screen when the UI is started</t>
+  </si>
+  <si>
+    <t>\Core\Main Display\Main Display\Actor Core.vi</t>
+  </si>
+  <si>
+    <t>Issue_006</t>
+  </si>
+  <si>
+    <t>Uninstallation of the package is not working well, the wrong components are attempted to be uninstalled from the LabVIEW Data directory</t>
+  </si>
+  <si>
+    <t>\VIP Build\Post-Uninstall Custom Action.vi</t>
+  </si>
+  <si>
+    <t>Issue_007</t>
+  </si>
+  <si>
+    <t>Create new assert UI does not default to the correct state when launched, sometimes off to the side</t>
+  </si>
+  <si>
+    <t>\Plugins\Utility\Build Assert VI.vi</t>
+  </si>
+  <si>
+    <t>Issue_008</t>
+  </si>
+  <si>
+    <t>Create assert memory tracking to shut down unused references</t>
+  </si>
+  <si>
+    <t>\Core\Assert API Components\Log Assert Core Components\Event Transmission\Get Failure Action Event.vi</t>
+  </si>
+  <si>
+    <t>Currently just opens a new event for each assert and never shuts them down until the application is closed, memory leak (but a small one)</t>
+  </si>
+  <si>
+    <t>Issue_009</t>
+  </si>
+  <si>
+    <t>Pause Application does not pause on the right spot</t>
+  </si>
+  <si>
+    <t>\Core\Assert API Components\Log Assert Core Components\Failure Actions\Pause Application\Action.vi</t>
+  </si>
+  <si>
+    <t>Issue_010</t>
+  </si>
+  <si>
+    <t>Create new assert UI takes too long to load</t>
+  </si>
+  <si>
+    <t>When a new assert is being created, the UI has to load dependencies each time and takes several seconds to load up.</t>
   </si>
 </sst>
 </file>
@@ -396,27 +462,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="147.140625" customWidth="1"/>
+    <col min="5" max="5" width="98.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -428,62 +494,191 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="C10">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F11">
+    <sortCondition ref="D2:D11"/>
+    <sortCondition ref="A2:A11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on Issue_017 to add options to create the assert vi inside or outside of the case structure. In order to get this working and do it properly, need to add in the json config file for the wizard and created a load of values in there.
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C2B0C8-5CF9-420F-9FDF-088EB61D6864}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F21EEE-0A98-4521-BBF1-44A14441DE49}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -142,6 +142,74 @@
   </si>
   <si>
     <t>When a new assert is being created, the UI has to load dependencies each time and takes several seconds to load up.</t>
+  </si>
+  <si>
+    <t>Solved by adding a simple local variable on startup for the tab control</t>
+  </si>
+  <si>
+    <t>Now working nicely.</t>
+  </si>
+  <si>
+    <t>Issue_011</t>
+  </si>
+  <si>
+    <t>Add the variant to data string function back to get data values added to the log file</t>
+  </si>
+  <si>
+    <t>\Core\Assert API Components\Log Assert Core Components\Failure Actions\Log To File\Action.vi</t>
+  </si>
+  <si>
+    <t>Issue_012</t>
+  </si>
+  <si>
+    <t>Only ever launch one instance of the dynamic filter window</t>
+  </si>
+  <si>
+    <t>\Core\Main Display\Main Display\Launch Dynamic Filter Window.vi</t>
+  </si>
+  <si>
+    <t>Issue_013</t>
+  </si>
+  <si>
+    <t>Add a UID to filters created so that the filter isn't overwritten if a new one is built with the same name</t>
+  </si>
+  <si>
+    <t>\Core\Filter Config Display\Filter Config Display\Filter Dialog.vi</t>
+  </si>
+  <si>
+    <t>Issue_014</t>
+  </si>
+  <si>
+    <t>Support multiple assert creation instead of just the first one in the array</t>
+  </si>
+  <si>
+    <t>Issue_015</t>
+  </si>
+  <si>
+    <t>Floating point numeric comparison precision is currently fixed</t>
+  </si>
+  <si>
+    <t>\Plugins\Utility\Convert to scripting configuration.vi</t>
+  </si>
+  <si>
+    <t>\Plugins\RCF Code\edit time panel and diagram\Assert API.llb\Assert API.vi
+\Plugins\QD Code\Scripting Code\Create New Assert.vi
+\Plugins\RCF Code\edit time panel and diagram\Assert API.llb\Execute Assert API.vi</t>
+  </si>
+  <si>
+    <t>Issue_016</t>
+  </si>
+  <si>
+    <t>add an option to insert new assert vi's on a fork rather than inline.</t>
+  </si>
+  <si>
+    <t>Issue_017</t>
+  </si>
+  <si>
+    <t>Add CDS outside of the assert vi (potentially in addition to the one inside or with a config file option)</t>
+  </si>
+  <si>
+    <t>\Plugins\Utility\Full Build Assert.vi</t>
   </si>
 </sst>
 </file>
@@ -165,7 +233,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -173,20 +241,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -462,223 +576,366 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="91.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2">
+      <c r="C12" s="1">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3">
+      <c r="C18" s="1">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
+      <c r="F18" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F11">
-    <sortCondition ref="D2:D11"/>
-    <sortCondition ref="A2:A11"/>
+  <sortState ref="A2:F18">
+    <sortCondition ref="D2:D18"/>
+    <sortCondition descending="1" ref="C2:C18"/>
+    <sortCondition ref="A2:A18"/>
   </sortState>
+  <conditionalFormatting sqref="A2:F2">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$D$2=Open</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="In Work">
+      <formula>NOT(ISERROR(SEARCH("In Work",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Worked on placement of asserts inside/outside CDS on the block diagram. Also sorting out the Wizard Config/config.json access
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F21EEE-0A98-4521-BBF1-44A14441DE49}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACBF9B4-9AFD-4A1D-A4BF-88ED2BCC01E9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6975" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -210,6 +210,43 @@
   </si>
   <si>
     <t>\Plugins\Utility\Full Build Assert.vi</t>
+  </si>
+  <si>
+    <t>Issue_018</t>
+  </si>
+  <si>
+    <t>Conditional disable is not deleted, no error</t>
+  </si>
+  <si>
+    <t>\Plugins\Utility\Delete CDS.vi</t>
+  </si>
+  <si>
+    <t>Does not generate an error - just doesn't do anything
+Turns out I was just being a dumbass!</t>
+  </si>
+  <si>
+    <t>I think this is getting close to being sorted now - need to test it and then fix all the crap that comes out….</t>
+  </si>
+  <si>
+    <t>In Work</t>
+  </si>
+  <si>
+    <t>Issue_019</t>
+  </si>
+  <si>
+    <t>Case structure to pull forked/inline setting from config file is Inline in both cases in the main UK</t>
+  </si>
+  <si>
+    <t>Issue_020</t>
+  </si>
+  <si>
+    <t>Numeric constant type change vi is erroring when building asserts</t>
+  </si>
+  <si>
+    <t>\Utility\Changes Constant Types.vi</t>
+  </si>
+  <si>
+    <t>Turned out it was because I put a CDS around everything in the templates and wasn't scanning with the Tref by label function - I was doing that for other changes. Now updated the code and it will work better. Build 1.0.0.14</t>
   </si>
 </sst>
 </file>
@@ -271,7 +308,124 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -576,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,32 +766,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1">
         <v>4</v>
@@ -646,7 +800,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>60</v>
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -825,114 +982,166 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="C14" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C15" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>39</v>
       </c>
     </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:F18">
-    <sortCondition ref="D2:D18"/>
-    <sortCondition descending="1" ref="C2:C18"/>
-    <sortCondition ref="A2:A18"/>
+  <sortState ref="A2:F20">
+    <sortCondition ref="D2:D20"/>
+    <sortCondition descending="1" ref="C2:C20"/>
+    <sortCondition ref="A2:A20"/>
   </sortState>
-  <conditionalFormatting sqref="A2:F2">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>$D$2=Open</formula>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>INDIRECT("D"&amp;ROW())="Solved"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",D1)))</formula>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>INDIRECT("d"&amp;ROW())="In Work"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="In Work">
-      <formula>NOT(ISERROR(SEARCH("In Work",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",D1)))</formula>
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>INDIRECT("D"&amp;ROW())="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working on Issue_023 and Issue_024. I think they should now be solved.
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACBF9B4-9AFD-4A1D-A4BF-88ED2BCC01E9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D70382C-102F-4C8C-A145-DC958BD06172}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6975" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="81">
   <si>
     <t>ID</t>
   </si>
@@ -247,6 +247,30 @@
   </si>
   <si>
     <t>Turned out it was because I put a CDS around everything in the templates and wasn't scanning with the Tref by label function - I was doing that for other changes. Now updated the code and it will work better. Build 1.0.0.14</t>
+  </si>
+  <si>
+    <t>Issue_021</t>
+  </si>
+  <si>
+    <t>Change "None" to "Display Only" in the failure actions enum</t>
+  </si>
+  <si>
+    <t>\Core\Assert API Components\Failure Actions.ctl</t>
+  </si>
+  <si>
+    <t>May have downstream effects which also have to be sorted out</t>
+  </si>
+  <si>
+    <t>Issue_022</t>
+  </si>
+  <si>
+    <t>Path for the CDS Structure vi is wrong</t>
+  </si>
+  <si>
+    <t>\Utility\CDS Placement Setup.vi</t>
+  </si>
+  <si>
+    <t>Change the relative path to "..\..\Templates\CDS Template\CDS Structure.vi"</t>
   </si>
 </sst>
 </file>
@@ -730,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,29 +830,32 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -837,15 +864,15 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -854,35 +881,32 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -890,16 +914,19 @@
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>43</v>
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -907,16 +934,16 @@
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -925,35 +952,32 @@
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1">
         <v>5</v>
@@ -961,16 +985,19 @@
       <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F12" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1">
         <v>5</v>
@@ -978,16 +1005,16 @@
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>12</v>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1">
         <v>5</v>
@@ -996,18 +1023,15 @@
         <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1">
         <v>5</v>
@@ -1016,122 +1040,162 @@
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="C16" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E16" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C17" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="C18" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C20" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>39</v>
+      <c r="E20" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>72</v>
+      <c r="E21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F20">
-    <sortCondition ref="D2:D20"/>
-    <sortCondition descending="1" ref="C2:C20"/>
-    <sortCondition ref="A2:A20"/>
+  <sortState ref="A2:F23">
+    <sortCondition ref="D2:D23"/>
+    <sortCondition descending="1" ref="C2:C23"/>
+    <sortCondition ref="A2:A23"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="expression" dxfId="5" priority="1">

</xml_diff>

<commit_message>
Found some big issues with changing the labels in the calling vi's CDS, think this is mostly sorted now by some modification to Rename Subdiagram Label.vi and building Find Labelled Disable Structure.vi. Added in Unit Tests/Find Disable Structure/Find Disable Structure/test - Find Disable Structure invalid.vi and Unit Tests/Find Disable Structure/Find Disable Structure/test - Find Disable Structure valid.vi to test it, they pass.
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D70382C-102F-4C8C-A145-DC958BD06172}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196018AA-4A57-4A89-9059-6C943EF102DF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9765" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="96">
   <si>
     <t>ID</t>
   </si>
@@ -271,6 +271,53 @@
   </si>
   <si>
     <t>Change the relative path to "..\..\Templates\CDS Template\CDS Structure.vi"</t>
+  </si>
+  <si>
+    <t>Issue_023</t>
+  </si>
+  <si>
+    <t>CDS in the templates is named different to the label searched for when deleting the CDS</t>
+  </si>
+  <si>
+    <t>\Utility\Delete CDS.vi</t>
+  </si>
+  <si>
+    <t>Issue_024</t>
+  </si>
+  <si>
+    <t>CDS is deleted during the edit time, but then the version called in the vi still contains it</t>
+  </si>
+  <si>
+    <t>Either change all the templates to "CDS" or change the label being searched for to "Conditional Disable Structure". Make sure it matches the CDS name in "CDS Template\CDS Structure.vi"</t>
+  </si>
+  <si>
+    <t>Something to do with the cache, not figured this one out yet - because the vi opens a new reference from file, its resaving the version on file rather than the version in memory. Change the "Save VI" functionality to gi the option of a reference or a file.</t>
+  </si>
+  <si>
+    <t>Issue_025</t>
+  </si>
+  <si>
+    <t>Change the templates to a single vim so changes to all can be easily applied</t>
+  </si>
+  <si>
+    <t>\Plugins\Templates</t>
+  </si>
+  <si>
+    <t>Such as renaming the CDS</t>
+  </si>
+  <si>
+    <t>Issue_026</t>
+  </si>
+  <si>
+    <t>Creating the label in the calling code causes an error 1055</t>
+  </si>
+  <si>
+    <t>\Utility\Add Evaluation String.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It should be added as a free label if the Assert is outside the CDS, or as a subdiagram label if it is inside the CDS. Believe this should be fixed in build version 1.0.0.18. Checking now. Found multiple reasons all contributing.
+"\Utility\Rename Subdiagram Label.vi" is in the wrong place, it is located after the vi has been inlined and the vi reference is therefore invalid.
+"\Utility\Rename Subdiagram Label.vi" is also not finding the conditional disable structure correctly. </t>
   </si>
 </sst>
 </file>
@@ -332,28 +379,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <b/>
@@ -384,97 +410,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -754,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +700,7 @@
     <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="98.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="91.5703125" style="2" customWidth="1"/>
   </cols>
@@ -790,24 +725,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="C2" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -903,30 +838,30 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -934,16 +869,19 @@
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>43</v>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -951,16 +889,16 @@
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -969,35 +907,32 @@
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>5</v>
@@ -1005,16 +940,19 @@
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F13" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1">
         <v>5</v>
@@ -1022,16 +960,16 @@
       <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>12</v>
+      <c r="F14" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1">
         <v>5</v>
@@ -1040,18 +978,15 @@
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C16" s="1">
         <v>5</v>
@@ -1060,15 +995,18 @@
         <v>15</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>
@@ -1077,18 +1015,15 @@
         <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -1097,114 +1032,194 @@
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C19" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="C20" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>55</v>
+      <c r="E20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C25" s="1">
         <v>3</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="D25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C26" s="1">
         <v>3</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="D26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C27" s="1">
         <v>2</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="D27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F23">
-    <sortCondition ref="D2:D23"/>
-    <sortCondition descending="1" ref="C2:C23"/>
-    <sortCondition ref="A2:A23"/>
+  <sortState ref="A2:F27">
+    <sortCondition ref="D2:D27"/>
+    <sortCondition descending="1" ref="C2:C27"/>
+    <sortCondition ref="A2:A27"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>INDIRECT("D"&amp;ROW())="Solved"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>INDIRECT("d"&amp;ROW())="In Work"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>INDIRECT("D"&amp;ROW())="Open"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Rearchitecting the process to insert an assert to the calling vi, building a state machine to allow the order to be reconfigured. Starting with an inline assert with the CDS inside the assert only, and no eval string (this is the simplest combination).
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196018AA-4A57-4A89-9059-6C943EF102DF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FC8C32-9C5D-420F-916F-7BF1305FAB75}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9765" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -315,9 +315,22 @@
     <t>\Utility\Add Evaluation String.vi</t>
   </si>
   <si>
-    <t xml:space="preserve">It should be added as a free label if the Assert is outside the CDS, or as a subdiagram label if it is inside the CDS. Believe this should be fixed in build version 1.0.0.18. Checking now. Found multiple reasons all contributing.
+    <t>It should be added as a free label if the Assert is outside the CDS, or as a subdiagram label if it is inside the CDS. Believe this should be fixed in build version 1.0.0.18. Checking now. Found multiple reasons all contributing.
 "\Utility\Rename Subdiagram Label.vi" is in the wrong place, it is located after the vi has been inlined and the vi reference is therefore invalid.
-"\Utility\Rename Subdiagram Label.vi" is also not finding the conditional disable structure correctly. </t>
+"\Utility\Rename Subdiagram Label.vi" is also not finding the conditional disable structure correctly. 
+Need to figure out the correct order of events, with the "Rename Subdiagram Label.vi" before deleting the outer vi, it fails in one configuration (outside/both) and the other way round it will fail in a different configuration.....</t>
+  </si>
+  <si>
+    <t>Issue_027</t>
+  </si>
+  <si>
+    <t>Make sure the confirm wire reference process will work fully with nested structures.</t>
+  </si>
+  <si>
+    <t>\Plugins\Utility\Confirm Wire Reference.vi</t>
+  </si>
+  <si>
+    <t>Build some unit tests to test if it will work first.</t>
   </si>
 </sst>
 </file>
@@ -689,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -858,30 +871,30 @@
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -889,16 +902,19 @@
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>43</v>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -906,16 +922,16 @@
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -924,35 +940,32 @@
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
         <v>5</v>
@@ -960,16 +973,19 @@
       <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F14" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1">
         <v>5</v>
@@ -977,16 +993,16 @@
       <c r="D15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>12</v>
+      <c r="F15" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1">
         <v>5</v>
@@ -995,18 +1011,15 @@
         <v>15</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>
@@ -1015,15 +1028,18 @@
         <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -1032,18 +1048,15 @@
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C19" s="1">
         <v>5</v>
@@ -1052,18 +1065,18 @@
         <v>15</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -1072,18 +1085,18 @@
         <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C21" s="1">
         <v>5</v>
@@ -1095,29 +1108,35 @@
         <v>83</v>
       </c>
       <c r="F21" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="1">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C22" s="1">
-        <v>4</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C23" s="1">
         <v>4</v>
@@ -1125,16 +1144,13 @@
       <c r="D23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C24" s="1">
         <v>4</v>
@@ -1142,36 +1158,36 @@
       <c r="D24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>65</v>
+      <c r="E24" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>6</v>
+      <c r="E25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C26" s="1">
         <v>3</v>
@@ -1179,38 +1195,55 @@
       <c r="D26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C28" s="1">
         <v>2</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="D28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F27">
-    <sortCondition ref="D2:D27"/>
-    <sortCondition descending="1" ref="C2:C27"/>
-    <sortCondition ref="A2:A27"/>
+  <sortState ref="A2:F28">
+    <sortCondition ref="D2:D28"/>
+    <sortCondition descending="1" ref="C2:C28"/>
+    <sortCondition ref="A2:A28"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="expression" dxfId="2" priority="1">

</xml_diff>

<commit_message>
Now have the first 2 states of the state machine in Process Insert Assert.vi working fine. Next two to add are the initial forked insertions.
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FC8C32-9C5D-420F-916F-7BF1305FAB75}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301CEBFF-F443-43E8-8A5C-AA17C13D9462}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9765" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
   <si>
     <t>ID</t>
   </si>
@@ -331,6 +331,15 @@
   </si>
   <si>
     <t>Build some unit tests to test if it will work first.</t>
+  </si>
+  <si>
+    <t>Issue_028</t>
+  </si>
+  <si>
+    <t>Free label drops as a floating object if the assert vi is inside a structure</t>
+  </si>
+  <si>
+    <t>\Utility\Add Free Label.vi</t>
   </si>
 </sst>
 </file>
@@ -702,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,30 +971,27 @@
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="C14" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1">
         <v>5</v>
@@ -993,16 +999,19 @@
       <c r="D15" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F15" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1">
         <v>5</v>
@@ -1010,16 +1019,16 @@
       <c r="D16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>12</v>
+      <c r="F16" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>
@@ -1028,18 +1037,15 @@
         <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -1048,15 +1054,18 @@
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1">
         <v>5</v>
@@ -1065,18 +1074,15 @@
         <v>15</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -1085,18 +1091,18 @@
         <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C21" s="1">
         <v>5</v>
@@ -1105,18 +1111,18 @@
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
@@ -1128,29 +1134,35 @@
         <v>83</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C23" s="1">
-        <v>4</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C24" s="1">
         <v>4</v>
@@ -1158,16 +1170,13 @@
       <c r="D24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C25" s="1">
         <v>4</v>
@@ -1175,36 +1184,36 @@
       <c r="D25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>65</v>
+      <c r="E25" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="C26" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>6</v>
+      <c r="E26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C27" s="1">
         <v>3</v>
@@ -1212,38 +1221,55 @@
       <c r="D27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="1">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C29" s="1">
         <v>2</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="D29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F28">
-    <sortCondition ref="D2:D28"/>
-    <sortCondition descending="1" ref="C2:C28"/>
-    <sortCondition ref="A2:A28"/>
+  <sortState ref="A2:F29">
+    <sortCondition ref="D2:D29"/>
+    <sortCondition descending="1" ref="C2:C29"/>
+    <sortCondition ref="A2:A29"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="expression" dxfId="2" priority="1">

</xml_diff>

<commit_message>
Changed the template vi's to vim's. Also had to go back to an old version of the VIP Build/Assert API.vipb file as it got corrupted.
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301CEBFF-F443-43E8-8A5C-AA17C13D9462}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB033E10-021E-4CCB-B8DD-F21935ACC266}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9765" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,19 +11,24 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$30</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="115">
   <si>
     <t>ID</t>
   </si>
@@ -226,9 +231,6 @@
   </si>
   <si>
     <t>I think this is getting close to being sorted now - need to test it and then fix all the crap that comes out….</t>
-  </si>
-  <si>
-    <t>In Work</t>
   </si>
   <si>
     <t>Issue_019</t>
@@ -340,6 +342,45 @@
   </si>
   <si>
     <t>\Utility\Add Free Label.vi</t>
+  </si>
+  <si>
+    <t>Issue_029</t>
+  </si>
+  <si>
+    <t>Adding a new assert doesn't seem to be doing it in a sensible position in the caller vi</t>
+  </si>
+  <si>
+    <t>\Utility\Process Insert Assert.vi</t>
+  </si>
+  <si>
+    <t>I think its worse when the Assert is placed inside a CDS on the caller block diagram</t>
+  </si>
+  <si>
+    <t>Issue_030</t>
+  </si>
+  <si>
+    <t>Rearchitec the section on comparison values to use a vim</t>
+  </si>
+  <si>
+    <t>\Utility\Process Build VI Operation.vi</t>
+  </si>
+  <si>
+    <t>zClosed</t>
+  </si>
+  <si>
+    <t>Issue_31</t>
+  </si>
+  <si>
+    <t>Use vim's for templates to reduce overhead</t>
+  </si>
+  <si>
+    <t>In work</t>
+  </si>
+  <si>
+    <t>\Utility\Build Assert VI.vi</t>
+  </si>
+  <si>
+    <t>Started off by changing all the current templates to vim's and will test it all still works. And then rationalise the number of templates down.</t>
   </si>
 </sst>
 </file>
@@ -401,7 +442,93 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -711,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,35 +874,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -783,36 +910,30 @@
       <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -821,15 +942,15 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -838,15 +959,18 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>89</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -855,55 +979,55 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>54</v>
+        <v>97</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>99</v>
+      <c r="E9" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -912,18 +1036,15 @@
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -931,16 +1052,16 @@
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>43</v>
+      <c r="E11" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -949,15 +1070,15 @@
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -966,32 +1087,38 @@
         <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>49</v>
+        <v>104</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>102</v>
+        <v>12</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1">
         <v>5</v>
@@ -999,19 +1126,16 @@
       <c r="D15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1">
         <v>5</v>
@@ -1019,16 +1143,16 @@
       <c r="D16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>19</v>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>
@@ -1037,15 +1161,18 @@
         <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>63</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -1054,18 +1181,15 @@
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C19" s="1">
         <v>5</v>
@@ -1074,15 +1198,18 @@
         <v>15</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -1091,18 +1218,18 @@
         <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C21" s="1">
         <v>5</v>
@@ -1111,18 +1238,18 @@
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
@@ -1131,18 +1258,18 @@
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C23" s="1">
         <v>5</v>
@@ -1151,10 +1278,10 @@
         <v>15</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1208,29 +1335,32 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="C27" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>6</v>
+      <c r="E27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C28" s="1">
         <v>3</v>
@@ -1238,48 +1368,105 @@
       <c r="D28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C30" s="1">
         <v>2</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="D30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>39</v>
       </c>
     </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="1">
+        <v>5</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:F29">
-    <sortCondition ref="D2:D29"/>
-    <sortCondition descending="1" ref="C2:C29"/>
-    <sortCondition ref="A2:A29"/>
+  <sortState ref="A2:F31">
+    <sortCondition ref="D2:D31"/>
+    <sortCondition descending="1" ref="C2:C31"/>
+    <sortCondition ref="A2:A31"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>INDIRECT("D"&amp;ROW())="Solved"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>INDIRECT("d"&amp;ROW())="In Work"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>INDIRECT("D"&amp;ROW())="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>INDIRECT("D"&amp;ROW())="zClosed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Starting to build up test classes to enable more flexibility without making the main configuration vi massively complex. Only done a small change so far to use a common template and then configure the additional data
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB033E10-021E-4CCB-B8DD-F21935ACC266}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFEAFDB-6CBA-4617-93BA-1CA20FB15D37}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9765" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11160" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="118">
   <si>
     <t>ID</t>
   </si>
@@ -368,9 +368,6 @@
     <t>zClosed</t>
   </si>
   <si>
-    <t>Issue_31</t>
-  </si>
-  <si>
     <t>Use vim's for templates to reduce overhead</t>
   </si>
   <si>
@@ -381,6 +378,18 @@
   </si>
   <si>
     <t>Started off by changing all the current templates to vim's and will test it all still works. And then rationalise the number of templates down.</t>
+  </si>
+  <si>
+    <t>Issue_031</t>
+  </si>
+  <si>
+    <t>Issue_032</t>
+  </si>
+  <si>
+    <t>Bin the inline insert</t>
+  </si>
+  <si>
+    <t>Stephen Loftus-Mercer recommends only adding asserts inline. Should be fairly simple, but will wait until I have the template reduction (Issue_031) sorted</t>
   </si>
 </sst>
 </file>
@@ -442,7 +451,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="4">
     <dxf>
       <font>
         <strike/>
@@ -450,82 +459,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -838,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,64 +809,70 @@
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>114</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="C2" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="C3" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -942,15 +881,15 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -959,18 +898,15 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -979,55 +915,55 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>43</v>
+      <c r="E9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -1036,15 +972,18 @@
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -1052,16 +991,16 @@
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>49</v>
+      <c r="E11" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1070,15 +1009,15 @@
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1087,55 +1026,52 @@
         <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>105</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>102</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="C15" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1">
         <v>5</v>
@@ -1146,13 +1082,16 @@
       <c r="E16" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F16" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>
@@ -1160,19 +1099,16 @@
       <c r="D17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -1181,15 +1117,15 @@
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C19" s="1">
         <v>5</v>
@@ -1198,18 +1134,18 @@
         <v>15</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -1218,18 +1154,15 @@
         <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C21" s="1">
         <v>5</v>
@@ -1238,18 +1171,18 @@
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
@@ -1258,18 +1191,18 @@
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C23" s="1">
         <v>5</v>
@@ -1278,49 +1211,58 @@
         <v>15</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C24" s="1">
-        <v>4</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="1">
-        <v>4</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C26" s="1">
         <v>4</v>
@@ -1328,19 +1270,13 @@
       <c r="D26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C27" s="1">
         <v>4</v>
@@ -1348,124 +1284,141 @@
       <c r="D27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>75</v>
+      <c r="E27" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="1">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C30" s="1">
         <v>3</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="D30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C31" s="1">
         <v>3</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C32" s="1">
         <v>2</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="D32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C33" s="1">
         <v>4</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" s="1">
-        <v>5</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:F31">
-    <sortCondition ref="D2:D31"/>
-    <sortCondition descending="1" ref="C2:C31"/>
-    <sortCondition ref="A2:A31"/>
+  <sortState ref="A2:F33">
+    <sortCondition ref="D2:D33"/>
+    <sortCondition descending="1" ref="C2:C33"/>
+    <sortCondition ref="A2:A33"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>INDIRECT("D"&amp;ROW())="Solved"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>INDIRECT("d"&amp;ROW())="In Work"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>INDIRECT("D"&amp;ROW())="Open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>INDIRECT("D"&amp;ROW())="zClosed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Investigating how to move more functionality into the Plugins/Utility/Test Classes/Configure test.vi core state machine, which is increasing the flexibility of the whole operation and adding to the flexible templates plan. Changing Build Evaluation String.vi and made the creation of that part of the Test.lvclass (haven't yet implemented any child classes so its a default string) Also changed the process for changing the icon colour to be part of the state machine.
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFEAFDB-6CBA-4617-93BA-1CA20FB15D37}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29963BA-495D-43EF-90EF-00F6962ADEA4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12555" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="121">
   <si>
     <t>ID</t>
   </si>
@@ -390,6 +390,15 @@
   </si>
   <si>
     <t>Stephen Loftus-Mercer recommends only adding asserts inline. Should be fairly simple, but will wait until I have the template reduction (Issue_031) sorted</t>
+  </si>
+  <si>
+    <t>Issue_033</t>
+  </si>
+  <si>
+    <t>Rearchitect Build Evaluation String to use the test class</t>
+  </si>
+  <si>
+    <t>\Plugins\Utility\Build Evaluation String.vi</t>
   </si>
 </sst>
 </file>
@@ -771,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,29 +876,29 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -898,15 +907,15 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -915,15 +924,15 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -932,18 +941,15 @@
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -952,38 +958,38 @@
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -991,16 +997,19 @@
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>43</v>
+      <c r="E11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1008,16 +1017,16 @@
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1026,15 +1035,15 @@
         <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -1043,15 +1052,15 @@
         <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -1060,38 +1069,35 @@
         <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="C16" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>
@@ -1099,16 +1105,19 @@
       <c r="D17" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F17" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -1116,16 +1125,16 @@
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>12</v>
+      <c r="F18" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1">
         <v>5</v>
@@ -1134,18 +1143,15 @@
         <v>15</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -1154,15 +1160,18 @@
         <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1">
         <v>5</v>
@@ -1171,18 +1180,15 @@
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
@@ -1191,18 +1197,18 @@
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C23" s="1">
         <v>5</v>
@@ -1211,18 +1217,18 @@
         <v>15</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
@@ -1234,15 +1240,15 @@
         <v>82</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C25" s="1">
         <v>5</v>
@@ -1251,32 +1257,38 @@
         <v>15</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C26" s="1">
-        <v>4</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C27" s="1">
         <v>4</v>
@@ -1284,16 +1296,13 @@
       <c r="D27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1">
         <v>4</v>
@@ -1301,19 +1310,16 @@
       <c r="D28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1">
         <v>4</v>
@@ -1322,35 +1328,38 @@
         <v>15</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="1">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="1">
-        <v>3</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C31" s="1">
         <v>3</v>
@@ -1358,55 +1367,72 @@
       <c r="D31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C33" s="1">
         <v>2</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="D33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C34" s="1">
         <v>4</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F33">
-    <sortCondition ref="D2:D33"/>
-    <sortCondition descending="1" ref="C2:C33"/>
-    <sortCondition ref="A2:A33"/>
+  <sortState ref="A2:F34">
+    <sortCondition ref="D2:D34"/>
+    <sortCondition descending="1" ref="C2:C34"/>
+    <sortCondition ref="A2:A34"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="expression" dxfId="3" priority="2">

</xml_diff>

<commit_message>
Modified the Configure test.vi to add the output so the evaluation string can be pulled from the test configuration JSON. I think this should pretty much be the flexible templates branch complete. Will build the package and test.
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29963BA-495D-43EF-90EF-00F6962ADEA4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED4EB2F-12BA-487C-BD36-443B805FE3D3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12555" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13950" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="124">
   <si>
     <t>ID</t>
   </si>
@@ -399,6 +399,15 @@
   </si>
   <si>
     <t>\Plugins\Utility\Build Evaluation String.vi</t>
+  </si>
+  <si>
+    <t>Issue_034</t>
+  </si>
+  <si>
+    <t>Add a default description and other parameters to the test configuration JSON string</t>
+  </si>
+  <si>
+    <t>Pretty simple to do</t>
   </si>
 </sst>
 </file>
@@ -780,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,50 +847,47 @@
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>38</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>118</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>119</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -890,32 +896,35 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="C6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -924,15 +933,15 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -941,15 +950,15 @@
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -958,18 +967,15 @@
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -978,38 +984,38 @@
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="C11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1017,16 +1023,19 @@
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>43</v>
+      <c r="E12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1034,16 +1043,16 @@
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -1052,15 +1061,15 @@
         <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -1069,15 +1078,15 @@
         <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
@@ -1086,38 +1095,35 @@
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="C17" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -1125,16 +1131,19 @@
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F18" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1">
         <v>5</v>
@@ -1142,16 +1151,16 @@
       <c r="D19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
+      <c r="F19" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -1160,18 +1169,15 @@
         <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C21" s="1">
         <v>5</v>
@@ -1180,15 +1186,18 @@
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
@@ -1197,18 +1206,15 @@
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C23" s="1">
         <v>5</v>
@@ -1217,18 +1223,18 @@
         <v>15</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
@@ -1237,18 +1243,18 @@
         <v>15</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C25" s="1">
         <v>5</v>
@@ -1260,15 +1266,15 @@
         <v>82</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C26" s="1">
         <v>5</v>
@@ -1277,32 +1283,38 @@
         <v>15</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C27" s="1">
-        <v>4</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C28" s="1">
         <v>4</v>
@@ -1310,16 +1322,13 @@
       <c r="D28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C29" s="1">
         <v>4</v>
@@ -1327,19 +1336,16 @@
       <c r="D29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C30" s="1">
         <v>4</v>
@@ -1348,35 +1354,38 @@
         <v>15</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1">
-        <v>3</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C32" s="1">
         <v>3</v>
@@ -1384,55 +1393,72 @@
       <c r="D32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C34" s="1">
         <v>2</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C35" s="1">
         <v>4</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F34">
-    <sortCondition ref="D2:D34"/>
-    <sortCondition descending="1" ref="C2:C34"/>
-    <sortCondition ref="A2:A34"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
+    <sortCondition ref="D2:D35"/>
+    <sortCondition descending="1" ref="C2:C35"/>
+    <sortCondition ref="A2:A35"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="expression" dxfId="3" priority="2">

</xml_diff>

<commit_message>
Started working on improving the UI speed - need to create a new branch for the next commit.
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED4EB2F-12BA-487C-BD36-443B805FE3D3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EB170D-0FEB-4E10-A114-ABE79E8FA5DB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13950" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15345" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,9 +371,6 @@
     <t>Use vim's for templates to reduce overhead</t>
   </si>
   <si>
-    <t>In work</t>
-  </si>
-  <si>
     <t>\Utility\Build Assert VI.vi</t>
   </si>
   <si>
@@ -408,6 +405,9 @@
   </si>
   <si>
     <t>Pretty simple to do</t>
+  </si>
+  <si>
+    <t>In Work</t>
   </si>
 </sst>
 </file>
@@ -792,7 +792,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,104 +827,101 @@
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>112</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>122</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>123</v>
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>117</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -933,89 +930,89 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>97</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>54</v>
+      <c r="E9" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1024,18 +1021,15 @@
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1043,87 +1037,93 @@
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>43</v>
+      <c r="E13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -1132,18 +1132,15 @@
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C19" s="1">
         <v>5</v>
@@ -1151,16 +1148,19 @@
       <c r="D19" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -1169,15 +1169,18 @@
         <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>12</v>
+        <v>78</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C21" s="1">
         <v>5</v>
@@ -1186,18 +1189,18 @@
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
@@ -1206,15 +1209,18 @@
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="C23" s="1">
         <v>5</v>
@@ -1223,18 +1229,18 @@
         <v>15</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
@@ -1243,18 +1249,18 @@
         <v>15</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="C25" s="1">
         <v>5</v>
@@ -1263,18 +1269,18 @@
         <v>15</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="C26" s="1">
         <v>5</v>
@@ -1282,39 +1288,30 @@
       <c r="D26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1">
         <v>4</v>
@@ -1322,13 +1319,16 @@
       <c r="D28" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E28" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1">
         <v>4</v>
@@ -1336,16 +1336,19 @@
       <c r="D29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1">
         <v>4</v>
@@ -1354,18 +1357,18 @@
         <v>15</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C31" s="1">
         <v>4</v>
@@ -1374,10 +1377,7 @@
         <v>15</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Part of the last commit
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED4EB2F-12BA-487C-BD36-443B805FE3D3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EB170D-0FEB-4E10-A114-ABE79E8FA5DB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13950" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15345" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,9 +371,6 @@
     <t>Use vim's for templates to reduce overhead</t>
   </si>
   <si>
-    <t>In work</t>
-  </si>
-  <si>
     <t>\Utility\Build Assert VI.vi</t>
   </si>
   <si>
@@ -408,6 +405,9 @@
   </si>
   <si>
     <t>Pretty simple to do</t>
+  </si>
+  <si>
+    <t>In Work</t>
   </si>
 </sst>
 </file>
@@ -792,7 +792,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,104 +827,101 @@
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>112</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>122</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>123</v>
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>117</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -933,89 +930,89 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>97</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>54</v>
+      <c r="E9" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1024,18 +1021,15 @@
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1043,87 +1037,93 @@
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>43</v>
+      <c r="E13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -1132,18 +1132,15 @@
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C19" s="1">
         <v>5</v>
@@ -1151,16 +1148,19 @@
       <c r="D19" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -1169,15 +1169,18 @@
         <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>12</v>
+        <v>78</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C21" s="1">
         <v>5</v>
@@ -1186,18 +1189,18 @@
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
@@ -1206,15 +1209,18 @@
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="C23" s="1">
         <v>5</v>
@@ -1223,18 +1229,18 @@
         <v>15</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
@@ -1243,18 +1249,18 @@
         <v>15</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="C25" s="1">
         <v>5</v>
@@ -1263,18 +1269,18 @@
         <v>15</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="C26" s="1">
         <v>5</v>
@@ -1282,39 +1288,30 @@
       <c r="D26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1">
         <v>4</v>
@@ -1322,13 +1319,16 @@
       <c r="D28" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E28" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1">
         <v>4</v>
@@ -1336,16 +1336,19 @@
       <c r="D29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1">
         <v>4</v>
@@ -1354,18 +1357,18 @@
         <v>15</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C31" s="1">
         <v>4</v>
@@ -1374,10 +1377,7 @@
         <v>15</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Working on improving UI speed - eliminating lots of unused code from the project to start with
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED4EB2F-12BA-487C-BD36-443B805FE3D3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EB170D-0FEB-4E10-A114-ABE79E8FA5DB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13950" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15345" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,9 +371,6 @@
     <t>Use vim's for templates to reduce overhead</t>
   </si>
   <si>
-    <t>In work</t>
-  </si>
-  <si>
     <t>\Utility\Build Assert VI.vi</t>
   </si>
   <si>
@@ -408,6 +405,9 @@
   </si>
   <si>
     <t>Pretty simple to do</t>
+  </si>
+  <si>
+    <t>In Work</t>
   </si>
 </sst>
 </file>
@@ -792,7 +792,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,104 +827,101 @@
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>112</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>122</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>123</v>
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>117</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -933,89 +930,89 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>97</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>54</v>
+      <c r="E9" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1024,18 +1021,15 @@
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1043,87 +1037,93 @@
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>43</v>
+      <c r="E13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -1132,18 +1132,15 @@
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C19" s="1">
         <v>5</v>
@@ -1151,16 +1148,19 @@
       <c r="D19" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -1169,15 +1169,18 @@
         <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>12</v>
+        <v>78</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C21" s="1">
         <v>5</v>
@@ -1186,18 +1189,18 @@
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
@@ -1206,15 +1209,18 @@
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="C23" s="1">
         <v>5</v>
@@ -1223,18 +1229,18 @@
         <v>15</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
@@ -1243,18 +1249,18 @@
         <v>15</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="C25" s="1">
         <v>5</v>
@@ -1263,18 +1269,18 @@
         <v>15</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="C26" s="1">
         <v>5</v>
@@ -1282,39 +1288,30 @@
       <c r="D26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1">
         <v>4</v>
@@ -1322,13 +1319,16 @@
       <c r="D28" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E28" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1">
         <v>4</v>
@@ -1336,16 +1336,19 @@
       <c r="D29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1">
         <v>4</v>
@@ -1354,18 +1357,18 @@
         <v>15</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C31" s="1">
         <v>4</v>
@@ -1374,10 +1377,7 @@
         <v>15</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LabVIEW has got confused
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EB170D-0FEB-4E10-A114-ABE79E8FA5DB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C978990A-1593-4A5C-AB42-2488E7008F09}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15345" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="16740" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$36</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="128">
   <si>
     <t>ID</t>
   </si>
@@ -408,6 +408,18 @@
   </si>
   <si>
     <t>In Work</t>
+  </si>
+  <si>
+    <t>Issue_035</t>
+  </si>
+  <si>
+    <t>Icon colours are no longer updating correctly</t>
+  </si>
+  <si>
+    <t>\Plugins\Utility\Set VI Icon Colour.vi</t>
+  </si>
+  <si>
+    <t>Used to work fine, I've broken it somehow</t>
   </si>
 </sst>
 </file>
@@ -789,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,12 +837,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>124</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="C2" s="1">
         <v>4</v>
@@ -839,10 +851,10 @@
         <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>126</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1306,12 +1318,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C28" s="1">
         <v>4</v>
@@ -1319,16 +1331,19 @@
       <c r="D28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>55</v>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C29" s="1">
         <v>4</v>
@@ -1336,19 +1351,16 @@
       <c r="D29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C30" s="1">
         <v>4</v>
@@ -1357,18 +1369,18 @@
         <v>15</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="C31" s="1">
         <v>4</v>
@@ -1377,32 +1389,35 @@
         <v>15</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="1">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="1">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C33" s="1">
         <v>3</v>
@@ -1410,55 +1425,77 @@
       <c r="D33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C35" s="1">
         <v>2</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="D35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C36" s="1">
         <v>4</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
-    <sortCondition ref="D2:D35"/>
-    <sortCondition descending="1" ref="C2:C35"/>
-    <sortCondition ref="A2:A35"/>
+  <autoFilter ref="A1:A36" xr:uid="{CCC54C03-2471-410E-B12D-0AF9752A92BE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F36">
+      <sortCondition ref="A1:A36"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F37">
+    <sortCondition ref="D2:D37"/>
+    <sortCondition descending="1" ref="C2:C37"/>
+    <sortCondition ref="A2:A37"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="expression" dxfId="3" priority="2">

</xml_diff>

<commit_message>
saved the Issue List/Issues.xlsx
</commit_message>
<xml_diff>
--- a/Issue List/Issues.xlsx
+++ b/Issue List/Issues.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EB170D-0FEB-4E10-A114-ABE79E8FA5DB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0869B858-6904-477F-83F7-3E4D6AF20408}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15345" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16740" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="127">
   <si>
     <t>ID</t>
   </si>
@@ -408,6 +408,15 @@
   </si>
   <si>
     <t>In Work</t>
+  </si>
+  <si>
+    <t>Issue_035</t>
+  </si>
+  <si>
+    <t>Remove the test/development mode settings from the post installation vi</t>
+  </si>
+  <si>
+    <t>\VIP Build\Post-Install Custom Action.vi</t>
   </si>
 </sst>
 </file>
@@ -789,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,22 +836,19 @@
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>124</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="C2" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1306,12 +1312,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C28" s="1">
         <v>4</v>
@@ -1319,16 +1325,19 @@
       <c r="D28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>55</v>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C29" s="1">
         <v>4</v>
@@ -1336,19 +1345,16 @@
       <c r="D29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C30" s="1">
         <v>4</v>
@@ -1357,18 +1363,18 @@
         <v>15</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="C31" s="1">
         <v>4</v>
@@ -1377,32 +1383,35 @@
         <v>15</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="1">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="1">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C33" s="1">
         <v>3</v>
@@ -1410,55 +1419,72 @@
       <c r="D33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C35" s="1">
         <v>2</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="D35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C36" s="1">
         <v>4</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
-    <sortCondition ref="D2:D35"/>
-    <sortCondition descending="1" ref="C2:C35"/>
-    <sortCondition ref="A2:A35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F36">
+    <sortCondition ref="D2:D36"/>
+    <sortCondition descending="1" ref="C2:C36"/>
+    <sortCondition ref="A2:A36"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="expression" dxfId="3" priority="2">

</xml_diff>